<commit_message>
added report to all tests
</commit_message>
<xml_diff>
--- a/Tests/OpenviduTests/test-input/Parameters.xlsx
+++ b/Tests/OpenviduTests/test-input/Parameters.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>TestName</t>
   </si>
@@ -22,7 +22,7 @@
     <t>NAMESESSION</t>
   </si>
   <si>
-    <t>TESTNAME</t>
+    <t>NAMEPARTICIPANT</t>
   </si>
   <si>
     <t>XpathJoinButton</t>
@@ -55,6 +55,21 @@
     <t>xpathHeader</t>
   </si>
   <si>
+    <t>idMainTitle</t>
+  </si>
+  <si>
+    <t>xpathSessionName</t>
+  </si>
+  <si>
+    <t>XpathParticipantName</t>
+  </si>
+  <si>
+    <t>idHeaderStartPage</t>
+  </si>
+  <si>
+    <t>xpathLeaveButton</t>
+  </si>
+  <si>
     <t>OpenViduJsTest</t>
   </si>
   <si>
@@ -104,6 +119,54 @@
   </si>
   <si>
     <t>/html/body/app-root/div/div/div[1]/img</t>
+  </si>
+  <si>
+    <t>OpenViduReactTest</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/</t>
+  </si>
+  <si>
+    <t>/html/body/div/div/div/div[3]/div[2]/div/div/video</t>
+  </si>
+  <si>
+    <t>//*[@id='main-video']/div/div/div/p</t>
+  </si>
+  <si>
+    <t>join</t>
+  </si>
+  <si>
+    <t>OpenViduVueTest</t>
+  </si>
+  <si>
+    <t>//*[@id='join-dialog']/div/p[3]/button</t>
+  </si>
+  <si>
+    <t>/html/body/div/div/div[3]/div[2]/video</t>
+  </si>
+  <si>
+    <t>//*[@id='main-video']/div/div/p</t>
+  </si>
+  <si>
+    <t>//*[@id='join-dialog']/div/p[2]/input</t>
+  </si>
+  <si>
+    <t>//*[@id='join-dialog']/div/p[1]/input</t>
+  </si>
+  <si>
+    <t>img-div</t>
+  </si>
+  <si>
+    <t>OpenViduHelloWordTest</t>
+  </si>
+  <si>
+    <t>//*[@id='join']/form/p[2]/input</t>
+  </si>
+  <si>
+    <t>/html/body/div[2]/div/div[2]/video</t>
+  </si>
+  <si>
+    <t>//*[@id='session']/input</t>
   </si>
 </sst>
 </file>
@@ -386,6 +449,10 @@
     <col customWidth="1" min="9" max="9" width="14.25"/>
     <col customWidth="1" min="11" max="11" width="15.75"/>
     <col customWidth="1" min="13" max="13" width="17.13"/>
+    <col customWidth="1" min="16" max="16" width="17.13"/>
+    <col customWidth="1" min="17" max="17" width="19.5"/>
+    <col customWidth="1" min="18" max="18" width="15.88"/>
+    <col customWidth="1" min="19" max="19" width="15.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -431,85 +498,217 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>30</v>
+      <c r="S6" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
     <hyperlink r:id="rId2" ref="B3"/>
+    <hyperlink r:id="rId3" ref="B4"/>
+    <hyperlink r:id="rId4" ref="B5"/>
+    <hyperlink r:id="rId5" ref="B6"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Delete innecesary files, updated function headers and updated OpenViduAngularTest
</commit_message>
<xml_diff>
--- a/Tests/OpenviduTests/test-input/Parameters.xlsx
+++ b/Tests/OpenviduTests/test-input/Parameters.xlsx
@@ -106,7 +106,7 @@
     <t>TestParticipant</t>
   </si>
   <si>
-    <t>/html/body/app-root/div/div/div[3]/div[2]/user-video/div/ov-video/video</t>
+    <t>/html/body/app-root/div/div/div[3]/div[2]/user-video/div/ov-video/video|//*[@id="remote-video-str_CAM_UiZU_con_RfF8HZtRaZ"]</t>
   </si>
   <si>
     <t>session-title</t>
@@ -216,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -225,6 +225,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -562,7 +565,7 @@
       <c r="F3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H3" s="2" t="s">

</xml_diff>